<commit_message>
Fix an acl statement issue Add Redis and use cache for JWT token
</commit_message>
<xml_diff>
--- a/doc/api.xlsx
+++ b/doc/api.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deviser\dev-doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Deviser\github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B85352F-3FD0-45E7-963E-DCD289B6353B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990AF3C3-1C8A-4432-B226-187ECEFA6546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="975" windowWidth="13800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="765" windowWidth="13800" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>IP Address</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>v1</t>
+  </si>
+  <si>
+    <t>Enable Redis</t>
   </si>
 </sst>
 </file>
@@ -434,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,12 +449,12 @@
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -459,13 +462,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -473,16 +476,16 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -490,7 +493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -498,15 +501,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -514,13 +517,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -533,8 +536,11 @@
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -547,10 +553,13 @@
       <c r="D14" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14:D14 B7:B8 B10" xr:uid="{DF15A493-BD64-49BE-9767-99D6D15A6EA4}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14:D14 B7:B10" xr:uid="{DF15A493-BD64-49BE-9767-99D6D15A6EA4}">
       <formula1>"No,Yes"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A14" xr:uid="{FC9C899F-6635-4382-A988-DF1E8A4C83CF}">

</xml_diff>

<commit_message>
Fix login API issue having unnecessary variables
</commit_message>
<xml_diff>
--- a/doc/api.xlsx
+++ b/doc/api.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Deviser\github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990AF3C3-1C8A-4432-B226-187ECEFA6546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABCB00-3E06-49DA-BA7C-ADC5C74C154D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="765" windowWidth="13800" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7965" yWindow="750" windowWidth="13800" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove empty start line in all files Add SMTP email template support
</commit_message>
<xml_diff>
--- a/doc/api.xlsx
+++ b/doc/api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Deviser\github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BABCB00-3E06-49DA-BA7C-ADC5C74C154D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C95ACE8-02A0-462E-AE5F-DF52E049BC54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="750" windowWidth="13800" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="885" windowWidth="13800" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>IP Address</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Enable Redis</t>
+  </si>
+  <si>
+    <t>Enable SMTP</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A13" sqref="A13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,59 +513,67 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14:D14 B7:B10" xr:uid="{DF15A493-BD64-49BE-9767-99D6D15A6EA4}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C15:D15 B7:B11" xr:uid="{DF15A493-BD64-49BE-9767-99D6D15A6EA4}">
       <formula1>"No,Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A14" xr:uid="{FC9C899F-6635-4382-A988-DF1E8A4C83CF}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A15" xr:uid="{FC9C899F-6635-4382-A988-DF1E8A4C83CF}">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>